<commit_message>
added latitudes for areas to allocation spreadsheet
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\07. Project-1\Project_Shark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\Documents\Bootcamp\Project_Shark\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71643D05-321F-4857-97AD-416037CE0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D273AFE6-2A80-4AF9-8F0E-EDC39C82D3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Output</t>
   </si>
@@ -172,6 +172,12 @@
   <si>
     <t>1. check https://catalogue.data.wa.gov.au to extract data from 2016 to 2020
 2, Possibly a heatmap on shark sightings</t>
+  </si>
+  <si>
+    <t>Latitude Yanchep</t>
+  </si>
+  <si>
+    <t>Latitude Dawsville</t>
   </si>
 </sst>
 </file>
@@ -209,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -232,17 +238,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,22 +591,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="100.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="68.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="47.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -607,8 +639,20 @@
       <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>-31.547102426001601</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2">
+        <v>-32.634355872262297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -625,7 +669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -640,7 +684,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -655,7 +699,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -670,7 +714,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -685,7 +729,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -700,7 +744,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -715,7 +759,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
added code for shark sightings, and shark news article
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\07. Project-1\Project_Shark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71643D05-321F-4857-97AD-416037CE0742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2FB00-833A-4B9E-8B71-3009149F1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -562,7 +563,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated code on shark_news (incl. Shark atk vs shark articles and shark attack vs activities
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\07. Project-1\Project_Shark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2FB00-833A-4B9E-8B71-3009149F1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2302335-46BB-43D0-ABA4-D9F773F35561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Output</t>
   </si>
   <si>
     <t>Variable</t>
-  </si>
-  <si>
-    <t>Heatmap: Shark</t>
   </si>
   <si>
     <t>Bar Chart: Shark attacks by Area</t>
@@ -94,9 +90,6 @@
   <si>
     <t>1. cleaning "Area" column in Shark Attack excel file
 2. Assigning "Fatality" score (i.e the higher, the deadlier) to assign weighting for the heatmap</t>
-  </si>
-  <si>
-    <t>Bar Chart: no. of shark stories in news in a year  vs total of shark attack count (do news cover all shark attacks?)</t>
   </si>
   <si>
     <t>Katherine</t>
@@ -111,14 +104,8 @@
     <t>Note</t>
   </si>
   <si>
-    <t>1. maybe around 5 groups? (i.e surfing, diving,, fishing,  Other) - TBA</t>
-  </si>
-  <si>
     <t>1. cleaning up the time column in shark attack data
 2. Grouping the time to Dawn (4am to 8am), Daytime (8am to 4pm)  Dusk (4pm to 8pm), Nightime (8pm to 4am)</t>
-  </si>
-  <si>
-    <t>Bar Chart: shark sightings vs shark attack (WA only)</t>
   </si>
   <si>
     <t>1. Filter excel file for 5 years data of car crash file
@@ -132,9 +119,6 @@
   </si>
   <si>
     <t>1. No. of days of stories of shark attacks</t>
-  </si>
-  <si>
-    <t>1. check abc news API to see if we can get a shark story</t>
   </si>
   <si>
     <t>1. no of shark sightings at a certain point in time
@@ -171,15 +155,41 @@
     <t>Kevin</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Heatmap: Shark Attack</t>
+  </si>
+  <si>
+    <t>Bar Chart &amp; Heatmap: shark sightings vs shark attack (WA only)</t>
+  </si>
+  <si>
     <t>1. check https://catalogue.data.wa.gov.au to extract data from 2016 to 2020
-2, Possibly a heatmap on shark sightings</t>
+2. Run a python API to extract latitude, longitude, sighting date, etc and save it as a CSV file
+3. Do a minor cleanup on CSV file via Excel to group up sightings based on year
+4. In Python, create a bar chart and a heatmap using the clean CSV file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Chart: no. of shark stories in news in a year  vs total of shark attack count </t>
+  </si>
+  <si>
+    <t>1. go to 9news.com.au and look for Shark Articles
+2. Use Parshub to extract all sharks related article into excel spreadsheet
+3. Do manual cleaning in Excel (adding year Column, manual check on relevancy of the article to shark attack, or whether the article is a repeat topic</t>
+  </si>
+  <si>
+    <t>1. Using the Shark Attacks excel spreadsheet, do a manual cleaning on the activity column by grouping up activities into smaller group
+2. run a bar chart to see the frequency of shark attacks based on human activities undertaken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +199,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,10 +251,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,8 +264,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,22 +581,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="100.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,156 +604,189 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <autoFilter ref="A1:F10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated kevin's code folder with newer code and also final presentation slide
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\07. Project-1\Project_Shark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2FB00-833A-4B9E-8B71-3009149F1601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2302335-46BB-43D0-ABA4-D9F773F35561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,15 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Output</t>
   </si>
   <si>
     <t>Variable</t>
-  </si>
-  <si>
-    <t>Heatmap: Shark</t>
   </si>
   <si>
     <t>Bar Chart: Shark attacks by Area</t>
@@ -94,9 +90,6 @@
   <si>
     <t>1. cleaning "Area" column in Shark Attack excel file
 2. Assigning "Fatality" score (i.e the higher, the deadlier) to assign weighting for the heatmap</t>
-  </si>
-  <si>
-    <t>Bar Chart: no. of shark stories in news in a year  vs total of shark attack count (do news cover all shark attacks?)</t>
   </si>
   <si>
     <t>Katherine</t>
@@ -111,14 +104,8 @@
     <t>Note</t>
   </si>
   <si>
-    <t>1. maybe around 5 groups? (i.e surfing, diving,, fishing,  Other) - TBA</t>
-  </si>
-  <si>
     <t>1. cleaning up the time column in shark attack data
 2. Grouping the time to Dawn (4am to 8am), Daytime (8am to 4pm)  Dusk (4pm to 8pm), Nightime (8pm to 4am)</t>
-  </si>
-  <si>
-    <t>Bar Chart: shark sightings vs shark attack (WA only)</t>
   </si>
   <si>
     <t>1. Filter excel file for 5 years data of car crash file
@@ -132,9 +119,6 @@
   </si>
   <si>
     <t>1. No. of days of stories of shark attacks</t>
-  </si>
-  <si>
-    <t>1. check abc news API to see if we can get a shark story</t>
   </si>
   <si>
     <t>1. no of shark sightings at a certain point in time
@@ -171,15 +155,41 @@
     <t>Kevin</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Heatmap: Shark Attack</t>
+  </si>
+  <si>
+    <t>Bar Chart &amp; Heatmap: shark sightings vs shark attack (WA only)</t>
+  </si>
+  <si>
     <t>1. check https://catalogue.data.wa.gov.au to extract data from 2016 to 2020
-2, Possibly a heatmap on shark sightings</t>
+2. Run a python API to extract latitude, longitude, sighting date, etc and save it as a CSV file
+3. Do a minor cleanup on CSV file via Excel to group up sightings based on year
+4. In Python, create a bar chart and a heatmap using the clean CSV file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Chart: no. of shark stories in news in a year  vs total of shark attack count </t>
+  </si>
+  <si>
+    <t>1. go to 9news.com.au and look for Shark Articles
+2. Use Parshub to extract all sharks related article into excel spreadsheet
+3. Do manual cleaning in Excel (adding year Column, manual check on relevancy of the article to shark attack, or whether the article is a repeat topic</t>
+  </si>
+  <si>
+    <t>1. Using the Shark Attacks excel spreadsheet, do a manual cleaning on the activity column by grouping up activities into smaller group
+2. run a bar chart to see the frequency of shark attacks based on human activities undertaken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +199,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,10 +251,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,8 +264,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,22 +581,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="100.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="68.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+    <col min="4" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="47.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,156 +604,189 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <autoFilter ref="A1:F10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>